<commit_message>
aktualisierung Zeitplan + Modelle + Teil der Kamerafahrtszene
</commit_message>
<xml_diff>
--- a/Zeitplan.xlsx
+++ b/Zeitplan.xlsx
@@ -5,11 +5,11 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Viktoria Horn\Documents\Studium\3. Semester\03Modul_Medienproduktion\3D-Modellierung und Animation\Projektphase\Nachts-im-Kinderzimmer\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\janak_000\Documents\HS Fulda\Semester 3\3DMA\Projekt\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7340"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7335"/>
   </bookViews>
   <sheets>
     <sheet name="Aufgabenliste Projekt 1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="86">
   <si>
     <t>Start:</t>
   </si>
@@ -284,6 +284,9 @@
   </si>
   <si>
     <t>(A) - Animation der Shots 10 - 14</t>
+  </si>
+  <si>
+    <t>13.12.</t>
   </si>
 </sst>
 </file>
@@ -1081,29 +1084,29 @@
   </sheetPr>
   <dimension ref="B1:I52"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="E46" sqref="E46"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="18.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="4" style="1" customWidth="1"/>
-    <col min="2" max="2" width="46.6328125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="14.26953125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="13.54296875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="16.1796875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="46.5703125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="14.28515625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="13.5703125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="16.140625" style="1" customWidth="1"/>
     <col min="6" max="6" width="15" style="1" customWidth="1"/>
-    <col min="7" max="7" width="21.90625" style="1" customWidth="1"/>
-    <col min="8" max="8" width="21.6328125" style="1" customWidth="1"/>
-    <col min="9" max="16384" width="9.1796875" style="1"/>
+    <col min="7" max="7" width="21.85546875" style="1" customWidth="1"/>
+    <col min="8" max="8" width="21.5703125" style="1" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="H1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="2:9" ht="4.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:9" ht="4.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
@@ -1114,12 +1117,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="2:9" ht="35.25" customHeight="1" x14ac:dyDescent="0.65">
+    <row r="3" spans="2:9" ht="35.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B3" s="26" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="2:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B5" s="6" t="s">
         <v>27</v>
       </c>
@@ -1130,22 +1133,21 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="2:9" s="2" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:9" s="2" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B6" s="29" t="s">
         <v>26</v>
       </c>
       <c r="C6" s="11"/>
       <c r="D6" s="12"/>
-      <c r="E6" s="28">
-        <f ca="1">TODAY()+27</f>
-        <v>42353</v>
+      <c r="E6" s="28" t="s">
+        <v>85</v>
       </c>
       <c r="F6" s="11"/>
       <c r="G6" s="27" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="8" spans="2:9" s="2" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:9" s="2" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B8" s="42" t="s">
         <v>28</v>
       </c>
@@ -1155,7 +1157,7 @@
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
     </row>
-    <row r="9" spans="2:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B9" s="13" t="s">
         <v>41</v>
       </c>
@@ -1181,7 +1183,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="2:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B10" s="13" t="s">
         <v>43</v>
       </c>
@@ -1203,7 +1205,7 @@
       </c>
       <c r="H10" s="15"/>
     </row>
-    <row r="11" spans="2:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B11" s="13" t="s">
         <v>34</v>
       </c>
@@ -1214,18 +1216,18 @@
         <v>38</v>
       </c>
       <c r="E11" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F11" s="16">
         <f>tblAufgabenliste[[#This Row],[% erledigt]]</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G11" s="13" t="s">
         <v>66</v>
       </c>
       <c r="H11" s="13"/>
     </row>
-    <row r="12" spans="2:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B12" s="13" t="s">
         <v>44</v>
       </c>
@@ -1236,18 +1238,18 @@
         <v>38</v>
       </c>
       <c r="E12" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F12" s="16">
         <f>tblAufgabenliste[[#This Row],[% erledigt]]</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G12" s="13" t="s">
         <v>67</v>
       </c>
       <c r="H12" s="13"/>
     </row>
-    <row r="13" spans="2:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B13" s="13" t="s">
         <v>46</v>
       </c>
@@ -1269,7 +1271,7 @@
       </c>
       <c r="H13" s="15"/>
     </row>
-    <row r="14" spans="2:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B14" s="13" t="s">
         <v>35</v>
       </c>
@@ -1280,18 +1282,18 @@
         <v>40</v>
       </c>
       <c r="E14" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F14" s="16">
         <f>tblAufgabenliste[[#This Row],[% erledigt]]</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G14" s="13" t="s">
         <v>69</v>
       </c>
       <c r="H14" s="13"/>
     </row>
-    <row r="15" spans="2:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B15" s="13" t="s">
         <v>36</v>
       </c>
@@ -1313,7 +1315,7 @@
       </c>
       <c r="H15" s="13"/>
     </row>
-    <row r="16" spans="2:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B16" s="13" t="s">
         <v>62</v>
       </c>
@@ -1335,7 +1337,7 @@
       </c>
       <c r="H16" s="13"/>
     </row>
-    <row r="17" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B17" s="13" t="s">
         <v>72</v>
       </c>
@@ -1345,17 +1347,19 @@
       <c r="D17" s="36" t="s">
         <v>39</v>
       </c>
-      <c r="E17" s="16"/>
+      <c r="E17" s="16">
+        <v>1</v>
+      </c>
       <c r="F17" s="16">
         <f>tblAufgabenliste[[#This Row],[% erledigt]]</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G17" s="13" t="s">
         <v>68</v>
       </c>
       <c r="H17" s="13"/>
     </row>
-    <row r="18" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B18" s="13" t="s">
         <v>73</v>
       </c>
@@ -1375,7 +1379,7 @@
       </c>
       <c r="H18" s="13"/>
     </row>
-    <row r="19" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B19" s="13" t="s">
         <v>50</v>
       </c>
@@ -1393,7 +1397,7 @@
       <c r="G19" s="13"/>
       <c r="H19" s="13"/>
     </row>
-    <row r="20" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B20" s="13" t="s">
         <v>51</v>
       </c>
@@ -1411,7 +1415,7 @@
       <c r="G20" s="13"/>
       <c r="H20" s="13"/>
     </row>
-    <row r="21" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B21" s="13" t="s">
         <v>71</v>
       </c>
@@ -1429,7 +1433,7 @@
       <c r="G21" s="13"/>
       <c r="H21" s="41"/>
     </row>
-    <row r="22" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B22" s="13" t="s">
         <v>52</v>
       </c>
@@ -1439,15 +1443,17 @@
       <c r="D22" s="36" t="s">
         <v>39</v>
       </c>
-      <c r="E22" s="16"/>
+      <c r="E22" s="16">
+        <v>1</v>
+      </c>
       <c r="F22" s="16">
         <f>tblAufgabenliste[[#This Row],[% erledigt]]</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G22" s="13"/>
       <c r="H22" s="13"/>
     </row>
-    <row r="23" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B23" s="37" t="s">
         <v>30</v>
       </c>
@@ -1467,7 +1473,7 @@
       <c r="G23" s="37"/>
       <c r="H23" s="37"/>
     </row>
-    <row r="24" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B24" s="13" t="s">
         <v>74</v>
       </c>
@@ -1487,7 +1493,7 @@
       <c r="G24" s="13"/>
       <c r="H24" s="13"/>
     </row>
-    <row r="25" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B25" s="13" t="s">
         <v>76</v>
       </c>
@@ -1507,7 +1513,7 @@
       <c r="G25" s="13"/>
       <c r="H25" s="13"/>
     </row>
-    <row r="26" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B26" s="13" t="s">
         <v>75</v>
       </c>
@@ -1527,7 +1533,7 @@
       <c r="G26" s="13"/>
       <c r="H26" s="13"/>
     </row>
-    <row r="27" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B27" s="13" t="s">
         <v>47</v>
       </c>
@@ -1547,7 +1553,7 @@
       <c r="G27" s="13"/>
       <c r="H27" s="13"/>
     </row>
-    <row r="28" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B28" s="13" t="s">
         <v>48</v>
       </c>
@@ -1567,7 +1573,7 @@
       <c r="G28" s="13"/>
       <c r="H28" s="13"/>
     </row>
-    <row r="29" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B29" s="13" t="s">
         <v>70</v>
       </c>
@@ -1587,7 +1593,7 @@
       <c r="G29" s="13"/>
       <c r="H29" s="13"/>
     </row>
-    <row r="30" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B30" s="13" t="s">
         <v>49</v>
       </c>
@@ -1607,7 +1613,7 @@
       <c r="G30" s="13"/>
       <c r="H30" s="13"/>
     </row>
-    <row r="31" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B31" s="13" t="s">
         <v>59</v>
       </c>
@@ -1627,7 +1633,7 @@
       <c r="G31" s="13"/>
       <c r="H31" s="13"/>
     </row>
-    <row r="32" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B32" s="13" t="s">
         <v>60</v>
       </c>
@@ -1647,7 +1653,7 @@
       <c r="G32" s="13"/>
       <c r="H32" s="13"/>
     </row>
-    <row r="33" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B33" s="13" t="s">
         <v>61</v>
       </c>
@@ -1667,7 +1673,7 @@
       <c r="G33" s="13"/>
       <c r="H33" s="13"/>
     </row>
-    <row r="34" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B34" s="13" t="s">
         <v>45</v>
       </c>
@@ -1687,7 +1693,7 @@
       <c r="G34" s="13"/>
       <c r="H34" s="13"/>
     </row>
-    <row r="35" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B35" s="13" t="s">
         <v>79</v>
       </c>
@@ -1707,7 +1713,7 @@
       <c r="G35" s="13"/>
       <c r="H35" s="41"/>
     </row>
-    <row r="36" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B36" s="13" t="s">
         <v>80</v>
       </c>
@@ -1727,7 +1733,7 @@
       <c r="G36" s="13"/>
       <c r="H36" s="41"/>
     </row>
-    <row r="37" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B37" s="37" t="s">
         <v>31</v>
       </c>
@@ -1747,7 +1753,7 @@
       <c r="G37" s="37"/>
       <c r="H37" s="37"/>
     </row>
-    <row r="38" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B38" s="13" t="s">
         <v>53</v>
       </c>
@@ -1767,7 +1773,7 @@
       <c r="G38" s="13"/>
       <c r="H38" s="13"/>
     </row>
-    <row r="39" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B39" s="13" t="s">
         <v>54</v>
       </c>
@@ -1787,7 +1793,7 @@
       <c r="G39" s="13"/>
       <c r="H39" s="13"/>
     </row>
-    <row r="40" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B40" s="13" t="s">
         <v>55</v>
       </c>
@@ -1807,7 +1813,7 @@
       <c r="G40" s="13"/>
       <c r="H40" s="13"/>
     </row>
-    <row r="41" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B41" s="13" t="s">
         <v>56</v>
       </c>
@@ -1827,7 +1833,7 @@
       <c r="G41" s="13"/>
       <c r="H41" s="13"/>
     </row>
-    <row r="42" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B42" s="13" t="s">
         <v>81</v>
       </c>
@@ -1847,7 +1853,7 @@
       <c r="G42" s="13"/>
       <c r="H42" s="13"/>
     </row>
-    <row r="43" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B43" s="13" t="s">
         <v>83</v>
       </c>
@@ -1867,7 +1873,7 @@
       <c r="G43" s="13"/>
       <c r="H43" s="41"/>
     </row>
-    <row r="44" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B44" s="13" t="s">
         <v>84</v>
       </c>
@@ -1887,7 +1893,7 @@
       <c r="G44" s="13"/>
       <c r="H44" s="41"/>
     </row>
-    <row r="45" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B45" s="37" t="s">
         <v>32</v>
       </c>
@@ -1907,7 +1913,7 @@
       <c r="G45" s="37"/>
       <c r="H45" s="37"/>
     </row>
-    <row r="46" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B46" s="13" t="s">
         <v>57</v>
       </c>
@@ -1927,7 +1933,7 @@
       <c r="G46" s="13"/>
       <c r="H46" s="13"/>
     </row>
-    <row r="47" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B47" s="13" t="s">
         <v>58</v>
       </c>
@@ -1947,7 +1953,7 @@
       <c r="G47" s="13"/>
       <c r="H47" s="41"/>
     </row>
-    <row r="48" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B48" s="13" t="s">
         <v>58</v>
       </c>
@@ -1967,7 +1973,7 @@
       <c r="G48" s="13"/>
       <c r="H48" s="41"/>
     </row>
-    <row r="49" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B49" s="13" t="s">
         <v>58</v>
       </c>
@@ -1987,7 +1993,7 @@
       <c r="G49" s="13"/>
       <c r="H49" s="13"/>
     </row>
-    <row r="50" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B50" s="13" t="s">
         <v>78</v>
       </c>
@@ -2007,7 +2013,7 @@
       <c r="G50" s="13"/>
       <c r="H50" s="13"/>
     </row>
-    <row r="51" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B51" s="13" t="s">
         <v>82</v>
       </c>
@@ -2027,7 +2033,7 @@
       <c r="G51" s="13"/>
       <c r="H51" s="41"/>
     </row>
-    <row r="52" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B52" s="37" t="s">
         <v>33</v>
       </c>
@@ -2132,17 +2138,17 @@
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="18.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="4" style="4" customWidth="1"/>
-    <col min="2" max="2" width="30.7265625" style="4" customWidth="1"/>
+    <col min="2" max="2" width="30.7109375" style="4" customWidth="1"/>
     <col min="3" max="3" width="40" style="4" customWidth="1"/>
-    <col min="4" max="4" width="32.26953125" style="4" customWidth="1"/>
-    <col min="5" max="5" width="36.26953125" style="4" customWidth="1"/>
-    <col min="6" max="16384" width="9.1796875" style="4"/>
+    <col min="4" max="4" width="32.28515625" style="4" customWidth="1"/>
+    <col min="5" max="5" width="36.28515625" style="4" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="4"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:6" s="1" customFormat="1" ht="4.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:6" s="1" customFormat="1" ht="4.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
@@ -2151,7 +2157,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="2:6" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="2:6" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B3" s="8" t="s">
         <v>6</v>
       </c>
@@ -2159,7 +2165,7 @@
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
     </row>
-    <row r="4" spans="2:6" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:6" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B4" s="44" t="s">
         <v>7</v>
       </c>
@@ -2167,7 +2173,7 @@
       <c r="D4" s="44"/>
       <c r="E4" s="44"/>
     </row>
-    <row r="5" spans="2:6" s="9" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:6" s="9" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B5" s="17" t="s">
         <v>8</v>
       </c>
@@ -2178,7 +2184,7 @@
         <v>Keine Hervorhebung</v>
       </c>
     </row>
-    <row r="6" spans="2:6" s="9" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:6" s="9" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B6" s="30" t="s">
         <v>9</v>
       </c>
@@ -2192,24 +2198,24 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="2:6" s="9" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:6" s="9" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B7" s="17" t="s">
         <v>15</v>
       </c>
       <c r="C7" s="18">
         <f ca="1">TODAY()-WEEKDAY(TODAY(),2)+1</f>
-        <v>42324</v>
+        <v>42331</v>
       </c>
       <c r="D7" s="18">
         <f ca="1">C7+6</f>
-        <v>42330</v>
+        <v>42337</v>
       </c>
       <c r="E7" s="19" t="str">
         <f ca="1">B7&amp;" ["&amp;TEXT(C7,"T MMM")&amp;" - "&amp;TEXT(D7,"T MMM")&amp;"]"</f>
-        <v xml:space="preserve">     Diese Woche [16 Nov - 22 Nov]</v>
-      </c>
-    </row>
-    <row r="8" spans="2:6" s="9" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v xml:space="preserve">     Diese Woche [23 Nov - 29 Nov]</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6" s="9" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B8" s="20" t="s">
         <v>16</v>
       </c>
@@ -2226,7 +2232,7 @@
         <v xml:space="preserve">     Dieser Monat [1 - 30, Nov]</v>
       </c>
     </row>
-    <row r="9" spans="2:6" s="9" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:6" s="9" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B9" s="17" t="s">
         <v>17</v>
       </c>
@@ -2243,7 +2249,7 @@
         <v xml:space="preserve">     Dieses Quartal [1 Apr - 31 Jul]</v>
       </c>
     </row>
-    <row r="10" spans="2:6" s="9" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:6" s="9" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B10" s="20" t="s">
         <v>18</v>
       </c>
@@ -2260,7 +2266,7 @@
         <v xml:space="preserve">     Dieses Jahr [2015]</v>
       </c>
     </row>
-    <row r="11" spans="2:6" s="9" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:6" s="9" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B11" s="34" t="s">
         <v>9</v>
       </c>
@@ -2271,24 +2277,24 @@
         <v>Intervall:</v>
       </c>
     </row>
-    <row r="12" spans="2:6" s="9" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:6" s="9" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B12" s="20" t="s">
         <v>19</v>
       </c>
       <c r="C12" s="22">
         <f ca="1">C7-7</f>
-        <v>42317</v>
+        <v>42324</v>
       </c>
       <c r="D12" s="22">
         <f ca="1">C12+6</f>
-        <v>42323</v>
+        <v>42330</v>
       </c>
       <c r="E12" s="21" t="str">
         <f ca="1">B12&amp;" ["&amp;TEXT(C12,"T MMM")&amp;" - "&amp;TEXT(D12,"T MMM")&amp;"]"</f>
-        <v xml:space="preserve">     Letzte Woche [9 Nov - 15 Nov]</v>
-      </c>
-    </row>
-    <row r="13" spans="2:6" s="9" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v xml:space="preserve">     Letzte Woche [16 Nov - 22 Nov]</v>
+      </c>
+    </row>
+    <row r="13" spans="2:6" s="9" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B13" s="17" t="s">
         <v>20</v>
       </c>
@@ -2305,7 +2311,7 @@
         <v xml:space="preserve">     Letzter Monat [1 - 31, Okt]</v>
       </c>
     </row>
-    <row r="14" spans="2:6" s="9" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:6" s="9" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B14" s="20" t="s">
         <v>21</v>
       </c>
@@ -2322,7 +2328,7 @@
         <v xml:space="preserve">     Letztes Quartal [1 Jan - 31 Mrz]</v>
       </c>
     </row>
-    <row r="15" spans="2:6" s="9" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:6" s="9" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B15" s="17" t="s">
         <v>22</v>
       </c>
@@ -2339,13 +2345,13 @@
         <v xml:space="preserve">     Letztes Jahr</v>
       </c>
     </row>
-    <row r="16" spans="2:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B16" s="20"/>
       <c r="C16" s="22"/>
       <c r="D16" s="22"/>
       <c r="E16" s="21"/>
     </row>
-    <row r="17" spans="2:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B17" s="35" t="s">
         <v>12</v>
       </c>
@@ -2362,7 +2368,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="2:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B18" s="20" t="s">
         <v>13</v>
       </c>
@@ -2373,7 +2379,7 @@
       <c r="D18" s="21"/>
       <c r="E18" s="21"/>
     </row>
-    <row r="19" spans="2:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B19" s="23" t="s">
         <v>14</v>
       </c>
@@ -2384,7 +2390,7 @@
       <c r="D19" s="24"/>
       <c r="E19" s="24"/>
     </row>
-    <row r="20" spans="2:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B20" s="10"/>
       <c r="C20" s="10"/>
       <c r="D20" s="10"/>

</xml_diff>